<commit_message>
fix 7888: fix set t1 to be t1u
</commit_message>
<xml_diff>
--- a/android_studio/guideMain/goluk_strings.xlsx
+++ b/android_studio/guideMain/goluk_strings.xlsx
@@ -28665,10 +28665,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -28691,16 +28691,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28715,9 +28722,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28729,29 +28751,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28766,10 +28766,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28783,7 +28791,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28797,11 +28805,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28814,22 +28829,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28850,7 +28850,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28862,7 +28874,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28874,25 +28922,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28910,7 +28940,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28922,25 +28994,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28952,19 +29012,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28976,61 +29024,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29059,30 +29059,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -29094,6 +29070,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -29115,11 +29100,44 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -29138,34 +29156,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -29174,133 +29174,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -29646,9 +29646,9 @@
   <dimension ref="A1:J1528"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1180" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1472" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E1184" sqref="E1184"/>
+      <selection pane="bottomLeft" activeCell="G1478" sqref="G1478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
7901:Crash if user hit save button frequently 7789:Rotate screen if video height bigger
</commit_message>
<xml_diff>
--- a/android_studio/guideMain/goluk_strings.xlsx
+++ b/android_studio/guideMain/goluk_strings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9575">
   <si>
     <t>name</t>
   </si>
@@ -19960,31 +19960,31 @@
     <t>set_ipc_item_hint_text</t>
   </si>
   <si>
-    <t>Sync the last wonderful and emergency videos automatically once connecting your phone with Goluk</t>
-  </si>
-  <si>
-    <t>手机与极路客连接成功后自动同步最近录制的精彩和紧急视频</t>
-  </si>
-  <si>
-    <t>當手機連接至極路客時，自動同步最近的精彩和危急情況紀錄影片</t>
-  </si>
-  <si>
-    <t>Synchroniser automatiquement les dernières vidéos magnifiques et d\'urgence après avoir connecté votre téléphone à Goluk</t>
-  </si>
-  <si>
-    <t>Die letzten wunderbaren Videos und Notfallvideos automatisch synchronisieren, sobald Ihr Mobiltelefon mit Goluk verbunden ist</t>
-  </si>
-  <si>
-    <t>Sincronizza automaticamente gli ultimi video meravigliosi e d\'emergenza quando connetti il telefono con Goluk</t>
-  </si>
-  <si>
-    <t>お使いの携帯をGolukと接続すると、最新のハイライトビデオと緊急ビデオ同期されます</t>
-  </si>
-  <si>
-    <t>휴대전화기를 Goluk에 연결하는 즉시 자동으로 최신 원더풀 및 비상 동영상 동기화</t>
-  </si>
-  <si>
-    <t>Автоматическая синхронизация последних замечательных и аварийных видеозаписей после подключения телефона к Goluk</t>
+    <t>Sync the last wonderful videos automatically once connecting your phone with Goluk</t>
+  </si>
+  <si>
+    <t>手机与极路客连接成功后自动同步最近录制的精彩</t>
+  </si>
+  <si>
+    <t>當手機連接至極路客時，自動同步最近的精彩紀錄影片</t>
+  </si>
+  <si>
+    <t>Synchroniser les dernières vidéos merveilleuses automatiquement une fois la connexion de votre téléphone avec Goluk</t>
+  </si>
+  <si>
+    <t>Synchronisieren Sie die letzten wunderbaren Videos automatisch, sobald Sie Ihr Handy mit Goluk verbinden</t>
+  </si>
+  <si>
+    <t>Sincronizza automaticamente gli ultimi video meravigliosi una volta connesso il telefono con Goluk</t>
+  </si>
+  <si>
+    <t>携帯電話とGolukを一度接続すれば、最後の素晴らしい動画を自動的に同期できます</t>
+  </si>
+  <si>
+    <t>휴대 전화를 Goluk에 연결하면 마지막 멋진 동영상을 자동으로 동기화 할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>Синхронизация последних замечательных видео автоматически после подключения телефона с Goluk</t>
   </si>
   <si>
     <t>my_install_title_text</t>
@@ -28709,6 +28709,9 @@
   </si>
   <si>
     <t>Идет экспорт видео, подождите...</t>
+  </si>
+  <si>
+    <t>signature_is_empty</t>
   </si>
   <si>
     <t>Signature cannot be empty</t>
@@ -28776,13 +28779,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -28790,14 +28786,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28812,7 +28809,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28820,7 +28817,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28834,19 +28845,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28866,8 +28868,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28890,7 +28893,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28898,9 +28901,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28934,61 +28937,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29006,7 +28955,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29024,19 +29033,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29054,61 +29111,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29167,6 +29170,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -29178,6 +29196,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -29202,30 +29229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -29246,10 +29249,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -29258,16 +29261,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -29279,16 +29282,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -29297,94 +29300,94 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -29748,9 +29751,9 @@
   <dimension ref="A1:J1529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1496" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1181" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H1505" sqref="H1505"/>
+      <selection pane="bottomLeft" activeCell="B1184" sqref="B1184:J1184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -61461,7 +61464,7 @@
         <v>6646</v>
       </c>
     </row>
-    <row r="1184" ht="102" spans="1:10">
+    <row r="1184" ht="89.25" spans="1:10">
       <c r="A1184" s="3" t="s">
         <v>6647</v>
       </c>
@@ -71801,33 +71804,36 @@
         <v>9564</v>
       </c>
     </row>
-    <row r="1529" ht="42.75" spans="2:10">
+    <row r="1529" ht="42.75" spans="1:10">
+      <c r="A1529" t="s">
+        <v>9565</v>
+      </c>
       <c r="B1529" s="3" t="s">
-        <v>9565</v>
+        <v>9566</v>
       </c>
       <c r="C1529" s="3" t="s">
-        <v>9566</v>
+        <v>9567</v>
       </c>
       <c r="D1529" t="s">
-        <v>9567</v>
+        <v>9568</v>
       </c>
       <c r="E1529" s="3" t="s">
-        <v>9568</v>
+        <v>9569</v>
       </c>
       <c r="F1529" s="3" t="s">
-        <v>9569</v>
+        <v>9570</v>
       </c>
       <c r="G1529" s="3" t="s">
-        <v>9570</v>
+        <v>9571</v>
       </c>
       <c r="H1529" s="3" t="s">
-        <v>9571</v>
+        <v>9572</v>
       </c>
       <c r="I1529" s="3" t="s">
-        <v>9572</v>
+        <v>9573</v>
       </c>
       <c r="J1529" s="3" t="s">
-        <v>9573</v>
+        <v>9574</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7944 : emergency video removed
</commit_message>
<xml_diff>
--- a/android_studio/guideMain/goluk_strings.xlsx
+++ b/android_studio/guideMain/goluk_strings.xlsx
@@ -19963,7 +19963,7 @@
     <t>Sync the last wonderful videos automatically once connecting your phone with Goluk</t>
   </si>
   <si>
-    <t>手机与极路客连接成功后自动同步最近录制的精彩</t>
+    <t>手机与极路客连接成功后自动同步最近录制的精彩视频</t>
   </si>
   <si>
     <t>當手機連接至極路客時，自動同步最近的精彩紀錄影片</t>
@@ -28747,9 +28747,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -28778,6 +28778,53 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -28786,7 +28833,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28808,61 +28891,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -28876,42 +28907,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -28937,19 +28937,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28961,7 +28997,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -28979,25 +29087,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29009,55 +29099,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29069,55 +29117,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -29147,6 +29147,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -29157,15 +29172,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -29203,8 +29209,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -29219,40 +29243,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -29261,133 +29261,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -29753,7 +29753,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1181" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B1184" sqref="B1184:J1184"/>
+      <selection pane="bottomLeft" activeCell="A1184" sqref="$A1184:$XFD1184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>